<commit_message>
Updated AkWarm and Heat Pump data in Library.
AkWarm 9/27/2018 Library, and October 15, 2018 NEEP Heat Pump Spreadsheet.
</commit_message>
<xml_diff>
--- a/data/city-util/raw/City Utility Links.xlsx
+++ b/data/city-util/raw/City Utility Links.xlsx
@@ -8,9 +8,11 @@
   </bookViews>
   <sheets>
     <sheet sheetId="1" r:id="rId1" name="City_Utility_Links"/>
+    <sheet r:id="rId4" sheetId="2" name="Misc_Info"/>
   </sheets>
   <definedNames>
     <definedName name="City_Utility_Links">'City_Utility_Links'!$A$1:$B$953</definedName>
+    <definedName name="Misc_Info">'Misc_Info'!$A$1:$H$2</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -49,6 +51,10 @@
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyProtection="1" applyNumberFormat="1" xfId="0">
+      <alignment wrapText="0" vertical="center" horizontal="general"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7982,4 +7988,89 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row outlineLevel="0" r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>LibVersion</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>DiscountRate</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>RegSurcharge</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>RegSurchargeElectric</t>
+        </is>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>PCEkWhLimit</t>
+        </is>
+      </c>
+      <c r="G1" s="0" t="inlineStr">
+        <is>
+          <t>PCEFundingPct</t>
+        </is>
+      </c>
+      <c r="H1" s="0" t="inlineStr">
+        <is>
+          <t>MiscNotes</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43370</v>
+      </c>
+      <c r="C2" s="0">
+        <v>2.99999993294477E-02</v>
+      </c>
+      <c r="D2" s="0">
+        <v>4.00000018998981E-03</v>
+      </c>
+      <c r="E2" s="0">
+        <v>9.77999996393919E-04</v>
+      </c>
+      <c r="F2" s="0">
+        <v>500</v>
+      </c>
+      <c r="G2" s="0">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="inlineStr">
+        <is>
+          <t>Inflation factors and discount rate from 2011 FEMP;  Regulatory surcharge is now correctly modeled as a % for gas utilities and a $/kWh surcharge for electric utilities.  PCE 100% funding in effect July 2018. Jan 2018 gas RCC is .40% of total bill - fuel costs use price before taxes added as program now does the math</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>